<commit_message>
added more test data for VSP test cases
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36A9052-CEA0-4EB8-A5F5-4F392A440024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803425F8-5942-47E7-9ED6-425794975EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="1140" windowWidth="21600" windowHeight="12735" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="6960" yWindow="2415" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
+    <sheet name="VerifyViewProfile" sheetId="2" r:id="rId2"/>
+    <sheet name="AddCCUI" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Result</t>
   </si>
@@ -224,6 +226,18 @@
   </si>
   <si>
     <t>This Profile will be deleted</t>
+  </si>
+  <si>
+    <t>Criteria</t>
+  </si>
+  <si>
+    <t>SearchBy</t>
+  </si>
+  <si>
+    <t>VerifyViewProfile</t>
+  </si>
+  <si>
+    <t>Name only</t>
   </si>
 </sst>
 </file>
@@ -602,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A47CD45-DA58-41BB-8932-1F85ED5AF22A}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,4 +880,268 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55D1ECD-C537-4674-BBA3-5DD834904B86}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C4E85C-1973-4098-937F-EB292CE7F7F3}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test data for Add and Delect CC
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803425F8-5942-47E7-9ED6-425794975EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C87EF5-6980-4156-AEC6-EB4B89EB9C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="2415" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="2760" yWindow="2235" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="4" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
     <sheet name="VerifyViewProfile" sheetId="2" r:id="rId2"/>
     <sheet name="AddCCUI" sheetId="3" r:id="rId3"/>
+    <sheet name="AddDeleteCCNotPrepopulated" sheetId="4" r:id="rId4"/>
+    <sheet name="AddDeleteCCPrepopulated" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="104">
   <si>
     <t>Result</t>
   </si>
@@ -238,6 +240,117 @@
   </si>
   <si>
     <t>Name only</t>
+  </si>
+  <si>
+    <t>FirstNameCC</t>
+  </si>
+  <si>
+    <t>MiddleNameCC</t>
+  </si>
+  <si>
+    <t>LastNameCC</t>
+  </si>
+  <si>
+    <t>SuffixCC</t>
+  </si>
+  <si>
+    <t>NickNameCC</t>
+  </si>
+  <si>
+    <t>CardNumberCC</t>
+  </si>
+  <si>
+    <t>ExpMonthCC</t>
+  </si>
+  <si>
+    <t>ExpYearCC</t>
+  </si>
+  <si>
+    <t>AL1CC</t>
+  </si>
+  <si>
+    <t>AL2CC</t>
+  </si>
+  <si>
+    <t>ZIPCC</t>
+  </si>
+  <si>
+    <t>ZIPExtCC</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Siefert</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>Tim MasterCard</t>
+  </si>
+  <si>
+    <t>5146312200000035</t>
+  </si>
+  <si>
+    <t>12- DEC</t>
+  </si>
+  <si>
+    <t>2028</t>
+  </si>
+  <si>
+    <t>365 Kanyakumari</t>
+  </si>
+  <si>
+    <t>Room 8</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>McCulumm</t>
+  </si>
+  <si>
+    <t>Brandon Amex</t>
+  </si>
+  <si>
+    <t>371449635392376</t>
+  </si>
+  <si>
+    <t>2225 Kendsha road</t>
+  </si>
+  <si>
+    <t>21093</t>
+  </si>
+  <si>
+    <t>All Fields CC</t>
+  </si>
+  <si>
+    <t>Required Fields CC</t>
+  </si>
+  <si>
+    <t>Delta Corp</t>
+  </si>
+  <si>
+    <t>This Profile is for Add CC</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t>Ross Discover</t>
+  </si>
+  <si>
+    <t>6011000993026909</t>
+  </si>
+  <si>
+    <t>1 - JAN</t>
+  </si>
+  <si>
+    <t>TitleCC</t>
   </si>
 </sst>
 </file>
@@ -616,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A47CD45-DA58-41BB-8932-1F85ED5AF22A}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:AH1048576"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C4E85C-1973-4098-937F-EB292CE7F7F3}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,4 +1257,577 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B1EDA5-E3A3-4794-9389-11A1BB516C67}">
+  <dimension ref="A1:AU3"/>
+  <sheetViews>
+    <sheetView topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC310AF0-6FFB-4A8E-A2F9-ECD1411C076E}">
+  <dimension ref="A1:AL2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test data for AddCreditCard
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C87EF5-6980-4156-AEC6-EB4B89EB9C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3851ADC-A828-469A-AA3F-01A29E947D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2235" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="4" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="2760" yWindow="2235" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="3" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B1EDA5-E3A3-4794-9389-11A1BB516C67}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AV1" sqref="AV1:AW1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC310AF0-6FFB-4A8E-A2F9-ECD1411C076E}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added test data for modify credit card
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3851ADC-A828-469A-AA3F-01A29E947D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF11252F-D2E2-4808-9420-86D7136C71EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2235" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="3" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="3990" yWindow="2790" windowWidth="21600" windowHeight="12735" tabRatio="893" activeTab="6" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="AddCCUI" sheetId="3" r:id="rId3"/>
     <sheet name="AddDeleteCCNotPrepopulated" sheetId="4" r:id="rId4"/>
     <sheet name="AddDeleteCCPrepopulated" sheetId="5" r:id="rId5"/>
+    <sheet name="CreateModifyDeleteProfile" sheetId="6" r:id="rId6"/>
+    <sheet name="AddModifyDeleteCC" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="144">
   <si>
     <t>Result</t>
   </si>
@@ -351,6 +353,126 @@
   </si>
   <si>
     <t>TitleCC</t>
+  </si>
+  <si>
+    <t>Quick Company</t>
+  </si>
+  <si>
+    <t>Lewinsky</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Garama</t>
+  </si>
+  <si>
+    <t>This Profile will be modified and deleted</t>
+  </si>
+  <si>
+    <t>ProfileNameMod</t>
+  </si>
+  <si>
+    <t>CompNameMod</t>
+  </si>
+  <si>
+    <t>TitleMod</t>
+  </si>
+  <si>
+    <t>FNameMod</t>
+  </si>
+  <si>
+    <t>MNameMod</t>
+  </si>
+  <si>
+    <t>LNameMod</t>
+  </si>
+  <si>
+    <t>SuffixMod</t>
+  </si>
+  <si>
+    <t>AL1Mod</t>
+  </si>
+  <si>
+    <t>AL2Mod</t>
+  </si>
+  <si>
+    <t>ZIPMod</t>
+  </si>
+  <si>
+    <t>ZIPExtMod</t>
+  </si>
+  <si>
+    <t>EmailMod</t>
+  </si>
+  <si>
+    <t>HomePhone1Mod</t>
+  </si>
+  <si>
+    <t>HomePhone2Mod</t>
+  </si>
+  <si>
+    <t>HomePhone3Mod</t>
+  </si>
+  <si>
+    <t>CommentsMod</t>
+  </si>
+  <si>
+    <t>ProfileNameModified</t>
+  </si>
+  <si>
+    <t>CompaneNameModified</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t>Bhaichung</t>
+  </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>Bhutia</t>
+  </si>
+  <si>
+    <t>Jr.</t>
+  </si>
+  <si>
+    <t>47 Sasha ct</t>
+  </si>
+  <si>
+    <t>Room 1</t>
+  </si>
+  <si>
+    <t>2587</t>
+  </si>
+  <si>
+    <t>iahmed2@govolution.com</t>
+  </si>
+  <si>
+    <t>603</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>3697</t>
+  </si>
+  <si>
+    <t>This Profile has been modified</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>ExpMonthCCMod</t>
+  </si>
+  <si>
+    <t>ExpYearCCMod</t>
+  </si>
+  <si>
+    <t>6 - JUN</t>
   </si>
 </sst>
 </file>
@@ -730,7 +852,7 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:AH3"/>
+      <selection activeCell="Y1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B1EDA5-E3A3-4794-9389-11A1BB516C67}">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+    <sheetView topLeftCell="AP1" workbookViewId="0">
       <selection activeCell="AV1" sqref="AV1:AW1048576"/>
     </sheetView>
   </sheetViews>
@@ -1573,8 +1695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC310AF0-6FFB-4A8E-A2F9-ECD1411C076E}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,4 +1952,614 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4940B053-892E-4D65-970C-387445E934F5}">
+  <dimension ref="A1:AX2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4C6E2C-C42D-471F-A066-CEBAB5BA432C}">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test data AddModifyDeleteACH
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF11252F-D2E2-4808-9420-86D7136C71EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298DF238-2C99-46DF-B52E-7DA28912FC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2790" windowWidth="21600" windowHeight="12735" tabRatio="893" activeTab="6" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="5460" yWindow="2805" windowWidth="21600" windowHeight="12735" tabRatio="893" firstSheet="2" activeTab="8" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="AddDeleteCCPrepopulated" sheetId="5" r:id="rId5"/>
     <sheet name="CreateModifyDeleteProfile" sheetId="6" r:id="rId6"/>
     <sheet name="AddModifyDeleteCC" sheetId="7" r:id="rId7"/>
+    <sheet name="AddACHMRF" sheetId="8" r:id="rId8"/>
+    <sheet name="AddModifyDeleteACH" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="164">
   <si>
     <t>Result</t>
   </si>
@@ -473,6 +475,66 @@
   </si>
   <si>
     <t>6 - JUN</t>
+  </si>
+  <si>
+    <t>This Profile is for Add ACH</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>RTN</t>
+  </si>
+  <si>
+    <t>NicknameACH</t>
+  </si>
+  <si>
+    <t>ACNumber</t>
+  </si>
+  <si>
+    <t>Personal Checking</t>
+  </si>
+  <si>
+    <t>Personal Savings</t>
+  </si>
+  <si>
+    <t>Business Checking</t>
+  </si>
+  <si>
+    <t>256072691</t>
+  </si>
+  <si>
+    <t>Ross PC</t>
+  </si>
+  <si>
+    <t>Ross PS</t>
+  </si>
+  <si>
+    <t>Ross Corp</t>
+  </si>
+  <si>
+    <t>25872222</t>
+  </si>
+  <si>
+    <t>25873333</t>
+  </si>
+  <si>
+    <t>25874444</t>
+  </si>
+  <si>
+    <t>NicknameACHMod</t>
+  </si>
+  <si>
+    <t>Ross PC Mod</t>
+  </si>
+  <si>
+    <t>Ross PS Mod</t>
+  </si>
+  <si>
+    <t>Ross Corp Mod</t>
+  </si>
+  <si>
+    <t>Required Fields ACH</t>
   </si>
 </sst>
 </file>
@@ -2293,8 +2355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4C6E2C-C42D-471F-A066-CEBAB5BA432C}">
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,4 +2624,657 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD29F020-32F0-46BA-9C78-0D5D38002911}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055BC8D0-1CFC-40D6-9313-A3584BAD2B30}">
+  <dimension ref="A1:AM4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test data for VSP Payments
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298DF238-2C99-46DF-B52E-7DA28912FC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DD1777-8F86-4CFA-BDB7-0251AA50147C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="2805" windowWidth="21600" windowHeight="12735" tabRatio="893" firstSheet="2" activeTab="8" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="893" firstSheet="2" activeTab="10" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="AddModifyDeleteCC" sheetId="7" r:id="rId7"/>
     <sheet name="AddACHMRF" sheetId="8" r:id="rId8"/>
     <sheet name="AddModifyDeleteACH" sheetId="9" r:id="rId9"/>
+    <sheet name="DC-CreateProfile" sheetId="10" r:id="rId10"/>
+    <sheet name="DC-CreateProfACH" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="200">
   <si>
     <t>Result</t>
   </si>
@@ -535,6 +537,114 @@
   </si>
   <si>
     <t>Required Fields ACH</t>
+  </si>
+  <si>
+    <t>Data Creation</t>
+  </si>
+  <si>
+    <t>PaymentsVisa</t>
+  </si>
+  <si>
+    <t>Tandon</t>
+  </si>
+  <si>
+    <t>Ravena</t>
+  </si>
+  <si>
+    <t>248 PhoolKaante road</t>
+  </si>
+  <si>
+    <t>This Profile is for Visa Payments</t>
+  </si>
+  <si>
+    <t>Tandon Visa</t>
+  </si>
+  <si>
+    <t>4012000098765439</t>
+  </si>
+  <si>
+    <t>PaymentsMC</t>
+  </si>
+  <si>
+    <t>PaymentsAmEx</t>
+  </si>
+  <si>
+    <t>PaymentsDI</t>
+  </si>
+  <si>
+    <t>MyMC Corp</t>
+  </si>
+  <si>
+    <t>MyAmEx Corp</t>
+  </si>
+  <si>
+    <t>MyVisa Corp</t>
+  </si>
+  <si>
+    <t>MyDI Corp</t>
+  </si>
+  <si>
+    <t>This Profile is for MC Payments</t>
+  </si>
+  <si>
+    <t>This Profile is for AmEx Payments</t>
+  </si>
+  <si>
+    <t>This Profile is for DI Payments</t>
+  </si>
+  <si>
+    <t>Tandon MC</t>
+  </si>
+  <si>
+    <t>Tandon AmEx</t>
+  </si>
+  <si>
+    <t>Tandon DI</t>
+  </si>
+  <si>
+    <t>PaymentsPC</t>
+  </si>
+  <si>
+    <t>PaymentsPS</t>
+  </si>
+  <si>
+    <t>PaymentsCorp</t>
+  </si>
+  <si>
+    <t>MyPC Corp</t>
+  </si>
+  <si>
+    <t>MyPS Corp</t>
+  </si>
+  <si>
+    <t>MyCorp Corp</t>
+  </si>
+  <si>
+    <t>This Profile is for Personal Checking Payments</t>
+  </si>
+  <si>
+    <t>This Profile is for Personal Savings Payments</t>
+  </si>
+  <si>
+    <t>This Profile is for Corporate Payments</t>
+  </si>
+  <si>
+    <t>Tandon PC</t>
+  </si>
+  <si>
+    <t>Tandon PS</t>
+  </si>
+  <si>
+    <t>Tandon Corp</t>
+  </si>
+  <si>
+    <t>30012222</t>
+  </si>
+  <si>
+    <t>30013333</t>
+  </si>
+  <si>
+    <t>30014444</t>
   </si>
 </sst>
 </file>
@@ -591,12 +701,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,6 +1290,975 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F32B79-CCE8-401C-87BF-7A6DD5C015A7}">
+  <dimension ref="A1:AL5"/>
+  <sheetViews>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.42578125" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DBA674-D846-4D8B-BA8C-1C7D34927EB0}">
+  <dimension ref="A1:AL4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1:AM1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.85546875" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55D1ECD-C537-4674-BBA3-5DD834904B86}">
   <dimension ref="A1:J2"/>
@@ -2355,7 +3435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4C6E2C-C42D-471F-A066-CEBAB5BA432C}">
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0">
       <selection activeCell="AA1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2806,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055BC8D0-1CFC-40D6-9313-A3584BAD2B30}">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added test data for search profile
</commit_message>
<xml_diff>
--- a/Bootstrap/VSP-Data.xlsx
+++ b/Bootstrap/VSP-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DD1777-8F86-4CFA-BDB7-0251AA50147C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CBC2D4-4679-4458-80B7-FC72DE44F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="893" firstSheet="2" activeTab="10" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="893" firstSheet="2" activeTab="11" xr2:uid="{F85E046C-D3FC-46F9-AA2F-5165245A7308}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProfile" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="AddModifyDeleteACH" sheetId="9" r:id="rId9"/>
     <sheet name="DC-CreateProfile" sheetId="10" r:id="rId10"/>
     <sheet name="DC-CreateProfACH" sheetId="11" r:id="rId11"/>
+    <sheet name="SearchProfile" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="214">
   <si>
     <t>Result</t>
   </si>
@@ -645,6 +646,48 @@
   </si>
   <si>
     <t>30014444</t>
+  </si>
+  <si>
+    <t>Address only</t>
+  </si>
+  <si>
+    <t>City only</t>
+  </si>
+  <si>
+    <t>ZIP/Postal Code</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>ProfileToBeSearched</t>
+  </si>
+  <si>
+    <t>Krushna Govinda</t>
+  </si>
+  <si>
+    <t>6801 Wilkower driveer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COCKEYSVILLE </t>
+  </si>
+  <si>
+    <t>21030</t>
+  </si>
+  <si>
+    <t>PTBS Company</t>
+  </si>
+  <si>
+    <t>411522633</t>
+  </si>
+  <si>
+    <t>imtiazstergosh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A47CD45-DA58-41BB-8932-1F85ED5AF22A}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,7 +1867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DBA674-D846-4D8B-BA8C-1C7D34927EB0}">
   <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AM1" sqref="AM1:AM1048576"/>
     </sheetView>
   </sheetViews>
@@ -2251,6 +2294,251 @@
       </c>
       <c r="AL4" s="1" t="s">
         <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9BF8E7-6E86-4CC0-BBC0-582817F79C94}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="24.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>